<commit_message>
Build a CORS Configuration file to Establish the connection Between FrontEnd and BackEnd
</commit_message>
<xml_diff>
--- a/carzone API.xlsx
+++ b/carzone API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybernxtsolutions-my.sharepoint.com/personal/vedant_patil_cybernxt_in/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swapnil Magare\Downloads\Carzone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0135E01-F971-4E49-BA1C-3EF8F6A36405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE02BDE0-8DDB-4614-8359-25131EB54974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B60F615C-9E17-4D64-BE69-ECF55DA8FD4C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Company</t>
   </si>
@@ -133,12 +133,63 @@
   <si>
     <t>http://localhost:8080/car/delete/5</t>
   </si>
+  <si>
+    <t>WORK</t>
+  </si>
+  <si>
+    <t>For fetching the Car Details by Car ID</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/car/model/Camry</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/car/model/{model}</t>
+  </si>
+  <si>
+    <t>For Updating Exsiting Car Details</t>
+  </si>
+  <si>
+    <t>For Deleting the car By ID</t>
+  </si>
+  <si>
+    <t>API Method</t>
+  </si>
+  <si>
+    <t>For Adding the Company</t>
+  </si>
+  <si>
+    <t>For Adding For Car for Company with companyd</t>
+  </si>
+  <si>
+    <t>For fetching the Car Details by Car Model name.</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/car  || http://localhost:8080/car?pageNumber=&amp;pageSize=10</t>
+  </si>
+  <si>
+    <t>For fetching the Car Details if you want you can give PageNumbe and PageSize</t>
+  </si>
+  <si>
+    <t>For fetching the Company Details by Company ID</t>
+  </si>
+  <si>
+    <t>For fetching tha Company Details by Company Name.</t>
+  </si>
+  <si>
+    <t>For fetching tha Company Details</t>
+  </si>
+  <si>
+    <t>For Updating Exsiting Company Details</t>
+  </si>
+  <si>
+    <t>For Deleting the Company By ID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +220,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +243,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -201,12 +266,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +336,28 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -545,177 +673,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44C7B91-9EFD-4AC2-8657-B42C922F04AE}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.33203125" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="37.5546875" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" customWidth="1"/>
+    <col min="1" max="1" width="47.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" customWidth="1"/>
+    <col min="4" max="4" width="38.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="58.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="39.21875" customWidth="1"/>
+    <col min="9" max="9" width="42.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="H4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="7" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="12"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="13" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{521FE792-9290-472E-926A-56675CE710DF}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{BE291BC9-19CB-40FE-8211-28D57EA7F794}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{4441A3B5-EA1F-4744-8B1D-14631E064B3E}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{E3A3A8DD-1EA0-4882-93AD-7EB6CB193835}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{BE7DD02F-475F-4D0E-B336-D46F5CDD67E4}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{222677A4-61C8-4E05-920D-097D76AD23B3}"/>
-    <hyperlink ref="C3" r:id="rId7" xr:uid="{D8AE465C-B973-48D3-B47A-0EFB7AFDA97D}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{A3117FD7-BF36-4AE8-8F31-E8F1F43303BB}"/>
-    <hyperlink ref="F2" r:id="rId9" xr:uid="{24B97EB7-A146-46D3-8C6C-9BF0BA01C606}"/>
-    <hyperlink ref="F3" r:id="rId10" xr:uid="{D58237EB-12D2-4B2B-8678-C8FD882A2197}"/>
-    <hyperlink ref="F4" r:id="rId11" xr:uid="{151344B7-4CAF-4F46-A56F-520B5CF639A6}"/>
-    <hyperlink ref="F5" r:id="rId12" xr:uid="{E2A041F7-13FD-42F8-8569-AC950984ED84}"/>
-    <hyperlink ref="F6" r:id="rId13" xr:uid="{AF7EF515-04AF-4467-9E46-79FEC539E1B3}"/>
-    <hyperlink ref="G3" r:id="rId14" xr:uid="{92F939B1-B547-4C9E-A013-3010A76030BA}"/>
-    <hyperlink ref="G4" r:id="rId15" xr:uid="{70D636EA-AF1B-4DEB-A7C3-44CCCE0CF72F}"/>
-    <hyperlink ref="G6" r:id="rId16" xr:uid="{4B5A5A4E-CBEE-4B97-A28D-2AD50E3E3A69}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{521FE792-9290-472E-926A-56675CE710DF}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{BE291BC9-19CB-40FE-8211-28D57EA7F794}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{4441A3B5-EA1F-4744-8B1D-14631E064B3E}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{E3A3A8DD-1EA0-4882-93AD-7EB6CB193835}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{BE7DD02F-475F-4D0E-B336-D46F5CDD67E4}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{222677A4-61C8-4E05-920D-097D76AD23B3}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{D8AE465C-B973-48D3-B47A-0EFB7AFDA97D}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{A3117FD7-BF36-4AE8-8F31-E8F1F43303BB}"/>
+    <hyperlink ref="H2" r:id="rId9" xr:uid="{24B97EB7-A146-46D3-8C6C-9BF0BA01C606}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{D58237EB-12D2-4B2B-8678-C8FD882A2197}"/>
+    <hyperlink ref="H5" r:id="rId11" display="http://localhost:8080/car" xr:uid="{151344B7-4CAF-4F46-A56F-520B5CF639A6}"/>
+    <hyperlink ref="H6" r:id="rId12" xr:uid="{E2A041F7-13FD-42F8-8569-AC950984ED84}"/>
+    <hyperlink ref="H7" r:id="rId13" xr:uid="{AF7EF515-04AF-4467-9E46-79FEC539E1B3}"/>
+    <hyperlink ref="I3" r:id="rId14" xr:uid="{92F939B1-B547-4C9E-A013-3010A76030BA}"/>
+    <hyperlink ref="I5" r:id="rId15" xr:uid="{70D636EA-AF1B-4DEB-A7C3-44CCCE0CF72F}"/>
+    <hyperlink ref="I7" r:id="rId16" xr:uid="{4B5A5A4E-CBEE-4B97-A28D-2AD50E3E3A69}"/>
+    <hyperlink ref="H4" r:id="rId17" xr:uid="{AC185714-C82B-4249-80B7-249840AA62CA}"/>
+    <hyperlink ref="I4" r:id="rId18" xr:uid="{70D54994-3D6C-46A7-A21B-63967CE651AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated carzone API.xlsx from Swapnil branch
</commit_message>
<xml_diff>
--- a/carzone API.xlsx
+++ b/carzone API.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swapnil Magare\Downloads\Carzone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE02BDE0-8DDB-4614-8359-25131EB54974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A678F8-141D-4CCF-BA5F-18B3723D5E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B60F615C-9E17-4D64-BE69-ECF55DA8FD4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Company" sheetId="1" r:id="rId1"/>
+    <sheet name="Car" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -312,12 +313,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -330,33 +330,60 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -676,7 +703,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +720,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -705,187 +732,119 @@
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="13" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
@@ -900,18 +859,139 @@
     <hyperlink ref="D5" r:id="rId6" xr:uid="{222677A4-61C8-4E05-920D-097D76AD23B3}"/>
     <hyperlink ref="D3" r:id="rId7" xr:uid="{D8AE465C-B973-48D3-B47A-0EFB7AFDA97D}"/>
     <hyperlink ref="D7" r:id="rId8" xr:uid="{A3117FD7-BF36-4AE8-8F31-E8F1F43303BB}"/>
-    <hyperlink ref="H2" r:id="rId9" xr:uid="{24B97EB7-A146-46D3-8C6C-9BF0BA01C606}"/>
-    <hyperlink ref="H3" r:id="rId10" xr:uid="{D58237EB-12D2-4B2B-8678-C8FD882A2197}"/>
-    <hyperlink ref="H5" r:id="rId11" display="http://localhost:8080/car" xr:uid="{151344B7-4CAF-4F46-A56F-520B5CF639A6}"/>
-    <hyperlink ref="H6" r:id="rId12" xr:uid="{E2A041F7-13FD-42F8-8569-AC950984ED84}"/>
-    <hyperlink ref="H7" r:id="rId13" xr:uid="{AF7EF515-04AF-4467-9E46-79FEC539E1B3}"/>
-    <hyperlink ref="I3" r:id="rId14" xr:uid="{92F939B1-B547-4C9E-A013-3010A76030BA}"/>
-    <hyperlink ref="I5" r:id="rId15" xr:uid="{70D636EA-AF1B-4DEB-A7C3-44CCCE0CF72F}"/>
-    <hyperlink ref="I7" r:id="rId16" xr:uid="{4B5A5A4E-CBEE-4B97-A28D-2AD50E3E3A69}"/>
-    <hyperlink ref="H4" r:id="rId17" xr:uid="{AC185714-C82B-4249-80B7-249840AA62CA}"/>
-    <hyperlink ref="I4" r:id="rId18" xr:uid="{70D54994-3D6C-46A7-A21B-63967CE651AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A06AC-6946-435A-925D-127D07C10ADE}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{479C453B-E271-4705-B84D-20B4A372C379}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{98F313C7-2B1D-494E-886B-BF5F151FD50F}"/>
+    <hyperlink ref="C5" r:id="rId3" display="http://localhost:8080/car" xr:uid="{23782BD3-50EC-4DDA-AB00-F9BDDE17B4AD}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{505865BE-C031-4EB3-8BDB-272019FD2CA5}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{90EF272E-10FD-4EB9-B019-FAAE8AABE416}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{8D6B077A-5113-4E06-945B-CD73DD8E17E6}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{784F080C-A673-4C79-8CCF-8A9E99FAC29A}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{B47E27D1-D33D-4310-8503-A817737D8832}"/>
+    <hyperlink ref="C4" r:id="rId9" xr:uid="{77AF12D5-E972-41A5-972D-259E6C3FD3BF}"/>
+    <hyperlink ref="D4" r:id="rId10" xr:uid="{4DE1032E-FAB8-4405-8BE5-C61FD3803A70}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the Excel file and UserController
</commit_message>
<xml_diff>
--- a/carzone API.xlsx
+++ b/carzone API.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swapnil Magare\Downloads\Carzone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A678F8-141D-4CCF-BA5F-18B3723D5E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C83D7C-B255-425E-9FEA-3D4F807BAD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B60F615C-9E17-4D64-BE69-ECF55DA8FD4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Company" sheetId="1" r:id="rId1"/>
-    <sheet name="Car" sheetId="2" r:id="rId2"/>
+    <sheet name="User" sheetId="3" r:id="rId1"/>
+    <sheet name="Company" sheetId="1" r:id="rId2"/>
+    <sheet name="Car" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Company</t>
   </si>
@@ -185,12 +185,95 @@
   <si>
     <t>For Deleting the Company By ID</t>
   </si>
+  <si>
+    <t>User / Admin</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/register</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/login?email=swapnil@gmail.com&amp;password=123</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/2</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/getAllUser</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/Update/status?id=1&amp;status=INACTIVE</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/logout?id=2</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/delete/2</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/login?email={email}&amp;password={password}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/Update?id={id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/Update/status?id={id}&amp;status={STATUS_ENUM}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/logout?id={ID}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/user/delete/{ID}</t>
+  </si>
+  <si>
+    <t>{
+  "name": "John Doe",
+  "email": "swapnil@gmail.com",
+  "phone": 1234567890,
+  "password": "123",
+  "role": "USER"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "name": "John Updated",
+  "email": "john.updated@example.com",
+  "phone": 1231231234,
+  "password": "newPassword123"
+}</t>
+  </si>
+  <si>
+    <t>Register the new User Or Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login by email and password for admin and user </t>
+  </si>
+  <si>
+    <t>Get perticular user details at Admin side and registered user only see his/her information</t>
+  </si>
+  <si>
+    <t>Get all user obly by Admin side.</t>
+  </si>
+  <si>
+    <t>User and Admin both can update there Information.</t>
+  </si>
+  <si>
+    <t>Admin can change Or block perticular user Access.</t>
+  </si>
+  <si>
+    <t>User and Admin logout</t>
+  </si>
+  <si>
+    <t>Admin can Remove a perticular user from database.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +314,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -365,26 +469,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -699,11 +812,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53487FB2-1D6F-4EEF-934F-C5F0AD5C46FD}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.77734375" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" customWidth="1"/>
+    <col min="3" max="3" width="84.21875" customWidth="1"/>
+    <col min="4" max="4" width="74.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="31" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{143EE2D6-26AA-4E96-BF94-90E640863F54}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{04339309-4BF1-496C-BC76-EAC89645D851}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{78AAE2DA-CCEF-424F-BDFF-233DD2409076}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{BF420228-747D-4306-B52F-2FABA2447C9A}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{3A8207B6-644B-4B2A-AEDF-0C806D154413}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{83E623C1-28E4-48F9-A265-CD9A21B30797}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{C94759CB-D6F6-44EE-AF85-0A5F8B14354B}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{D0535319-0B09-4292-8C0D-5A7E7A63C92E}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{36A5AA65-D0D1-4FED-8D01-4D970270FA4E}"/>
+    <hyperlink ref="D3" r:id="rId10" xr:uid="{FE62A1B0-75FB-4F44-AC19-085DF8A3172C}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{6EA2558B-6A61-4B7B-B999-813DFCB643A1}"/>
+    <hyperlink ref="D6" r:id="rId12" display="http://localhost:8080/user/Update?id=1" xr:uid="{E49EA76E-AB84-4321-AEAF-8BC5AE6294D1}"/>
+    <hyperlink ref="D5" r:id="rId13" xr:uid="{85FEE3AD-779C-4F17-9172-C02A399FED11}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{79F9A4A3-1BA7-415C-B909-7E88D9FA03EA}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{B1DF3052-2F0A-4AEB-ACC3-42DC82209D7C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44C7B91-9EFD-4AC2-8657-B42C922F04AE}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,9 +1017,9 @@
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -752,10 +1035,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -771,8 +1054,8 @@
         <v>13</v>
       </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="27"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
@@ -784,8 +1067,8 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="27"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
@@ -803,9 +1086,9 @@
         <v>7</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -822,10 +1105,10 @@
         <v>15</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -841,8 +1124,8 @@
         <v>14</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="27"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
     </row>
@@ -865,13 +1148,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A06AC-6946-435A-925D-127D07C10ADE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>